<commit_message>
Update: README, testing details
</commit_message>
<xml_diff>
--- a/Flight-Management-API-Design-Sample.xlsx
+++ b/Flight-Management-API-Design-Sample.xlsx
@@ -520,15 +520,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -544,7 +544,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -646,6 +646,48 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>657000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>916920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4705920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>3231360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19739880" y="1186200"/>
+          <a:ext cx="4048920" cy="2314440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -761,8 +803,8 @@
   </sheetPr>
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -775,7 +817,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="36.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="53.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="3" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="66.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="3" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -822,7 +865,7 @@
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="316.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="315.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -959,6 +1002,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -969,7 +1013,7 @@
   </sheetPr>
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>